<commit_message>
add mark as read + download excel
</commit_message>
<xml_diff>
--- a/data.xlsx.xlsx
+++ b/data.xlsx.xlsx
@@ -7539,14 +7539,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8034,13 +8027,16 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -8049,118 +8045,115 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -8168,13 +8161,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8710,8 +8703,8 @@
   <sheetPr/>
   <dimension ref="A1:N570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>